<commit_message>
remise à jour de la spec avec les tests réussis
</commit_message>
<xml_diff>
--- a/DefinitionEtSuiviDeTaches-v02.xlsx
+++ b/DefinitionEtSuiviDeTaches-v02.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC-i7-Julien\Desktop\cours\ps5\division tâches\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC-i7-Julien\Documents\GitHub\ps5-GroupeK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{79F88755-4ABB-4DC9-88DA-31B41CCCE823}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F59B9486-71CC-492B-B43D-FAB3165B2F82}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -315,7 +315,24 @@
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="51">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1040,7 +1057,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1180,7 +1197,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1523,7 +1540,7 @@
       </c>
       <c r="C22" s="9">
         <f>COUNTIFS($F$3:$F$16,B22,$J$3:$J$16,"=OK")/COUNTIF($F$3:$F$16,B22)</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1578,77 +1595,72 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="G6:G9">
-    <cfRule type="containsText" dxfId="48" priority="84" operator="containsText" text="PF">
+    <cfRule type="containsText" dxfId="50" priority="86" operator="containsText" text="PF">
       <formula>NOT(ISERROR(SEARCH("PF",G6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3">
-    <cfRule type="containsText" dxfId="47" priority="81" operator="containsText" text="NOK">
+    <cfRule type="containsText" dxfId="49" priority="83" operator="containsText" text="NOK">
       <formula>NOT(ISERROR(SEARCH("NOK",J3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:G3 D6:G8 D7:F18 G6:G9 F4:F5 A19:G19 A28:G1048576 A20:B26 B8:B18 C20:G27">
-    <cfRule type="cellIs" dxfId="46" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="87" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:J3 H19:J1048576 H6:I18">
-    <cfRule type="cellIs" dxfId="45" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="84" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="containsText" dxfId="44" priority="79" operator="containsText" text="PF">
+    <cfRule type="containsText" dxfId="46" priority="81" operator="containsText" text="PF">
       <formula>NOT(ISERROR(SEARCH("PF",G4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J5">
-    <cfRule type="containsText" dxfId="43" priority="77" operator="containsText" text="NOK">
-      <formula>NOT(ISERROR(SEARCH("NOK",J5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C6:G6 B6:F7 C6:C18 B4:E5 G4:G5">
-    <cfRule type="cellIs" dxfId="42" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="82" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:J5 H4:I7">
-    <cfRule type="cellIs" dxfId="41" priority="78" operator="equal">
+  <conditionalFormatting sqref="H4:I7">
+    <cfRule type="cellIs" dxfId="43" priority="80" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A18">
-    <cfRule type="cellIs" dxfId="40" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="75" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:J18">
-    <cfRule type="containsText" dxfId="39" priority="65" operator="containsText" text="NOK">
+    <cfRule type="containsText" dxfId="41" priority="67" operator="containsText" text="NOK">
       <formula>NOT(ISERROR(SEARCH("NOK",J16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:J18">
+    <cfRule type="cellIs" dxfId="40" priority="68" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8:G18">
+    <cfRule type="containsText" dxfId="39" priority="65" operator="containsText" text="PF">
+      <formula>NOT(ISERROR(SEARCH("PF",G8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8:G18">
     <cfRule type="cellIs" dxfId="38" priority="66" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G8:G18">
-    <cfRule type="containsText" dxfId="37" priority="63" operator="containsText" text="PF">
-      <formula>NOT(ISERROR(SEARCH("PF",G8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G8:G18">
-    <cfRule type="cellIs" dxfId="36" priority="64" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="35" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="62" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C27">
-    <cfRule type="dataBar" priority="88">
+    <cfRule type="dataBar" priority="90">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -1660,7 +1672,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="dataBar" priority="89">
+    <cfRule type="dataBar" priority="91">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1674,176 +1686,166 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="containsText" dxfId="34" priority="52" operator="containsText" text="PF">
+    <cfRule type="containsText" dxfId="36" priority="54" operator="containsText" text="PF">
       <formula>NOT(ISERROR(SEARCH("PF",G5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="33" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="48" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J5">
-    <cfRule type="containsText" dxfId="32" priority="44" operator="containsText" text="NOK">
-      <formula>NOT(ISERROR(SEARCH("NOK",J5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J5">
-    <cfRule type="cellIs" dxfId="31" priority="45" operator="equal">
+  <conditionalFormatting sqref="G5">
+    <cfRule type="containsText" dxfId="32" priority="45" operator="containsText" text="PF">
+      <formula>NOT(ISERROR(SEARCH("PF",G5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6">
+    <cfRule type="cellIs" dxfId="31" priority="39" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6">
+    <cfRule type="containsText" dxfId="28" priority="36" operator="containsText" text="PF">
+      <formula>NOT(ISERROR(SEARCH("PF",G6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J6">
+    <cfRule type="containsText" dxfId="27" priority="19" operator="containsText" text="NOK">
+      <formula>NOT(ISERROR(SEARCH("NOK",J6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J6">
+    <cfRule type="cellIs" dxfId="26" priority="20" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5">
-    <cfRule type="containsText" dxfId="30" priority="43" operator="containsText" text="PF">
-      <formula>NOT(ISERROR(SEARCH("PF",G5)))</formula>
+  <conditionalFormatting sqref="G7">
+    <cfRule type="cellIs" dxfId="25" priority="30" operator="equal">
+      <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="29" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J5">
-    <cfRule type="containsText" dxfId="28" priority="35" operator="containsText" text="NOK">
-      <formula>NOT(ISERROR(SEARCH("NOK",J5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J5">
-    <cfRule type="cellIs" dxfId="27" priority="36" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="containsText" dxfId="26" priority="34" operator="containsText" text="PF">
-      <formula>NOT(ISERROR(SEARCH("PF",G6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J6">
-    <cfRule type="containsText" dxfId="25" priority="17" operator="containsText" text="NOK">
-      <formula>NOT(ISERROR(SEARCH("NOK",J6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J6">
-    <cfRule type="cellIs" dxfId="24" priority="18" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G7">
-    <cfRule type="cellIs" dxfId="23" priority="28" operator="equal">
+  <conditionalFormatting sqref="G15">
+    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="PF">
+      <formula>NOT(ISERROR(SEARCH("PF",G15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G15">
+    <cfRule type="cellIs" dxfId="22" priority="26" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="22" priority="25" operator="equal">
-      <formula>"F"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G15">
+  <conditionalFormatting sqref="G11">
     <cfRule type="containsText" dxfId="21" priority="23" operator="containsText" text="PF">
-      <formula>NOT(ISERROR(SEARCH("PF",G15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G15">
+      <formula>NOT(ISERROR(SEARCH("PF",G11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
     <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G11">
-    <cfRule type="containsText" dxfId="19" priority="21" operator="containsText" text="PF">
-      <formula>NOT(ISERROR(SEARCH("PF",G11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G11">
+  <conditionalFormatting sqref="J4">
+    <cfRule type="containsText" dxfId="19" priority="21" operator="containsText" text="NOK">
+      <formula>NOT(ISERROR(SEARCH("NOK",J4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J4">
     <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
-      <formula>"F"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J4">
-    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="NOK">
-      <formula>NOT(ISERROR(SEARCH("NOK",J4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7">
+    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="NOK">
+      <formula>NOT(ISERROR(SEARCH("NOK",J7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J7">
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J8">
     <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="NOK">
-      <formula>NOT(ISERROR(SEARCH("NOK",J7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J7">
+      <formula>NOT(ISERROR(SEARCH("NOK",J8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J8">
     <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J8">
+  <conditionalFormatting sqref="J9">
     <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="NOK">
-      <formula>NOT(ISERROR(SEARCH("NOK",J8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J8">
+      <formula>NOT(ISERROR(SEARCH("NOK",J9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9">
     <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J9">
+  <conditionalFormatting sqref="J10:J11">
     <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="NOK">
-      <formula>NOT(ISERROR(SEARCH("NOK",J9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J9">
+      <formula>NOT(ISERROR(SEARCH("NOK",J10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10:J11">
     <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J10:J11">
+  <conditionalFormatting sqref="J12">
     <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="NOK">
-      <formula>NOT(ISERROR(SEARCH("NOK",J10)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J10:J11">
+      <formula>NOT(ISERROR(SEARCH("NOK",J12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J12">
     <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J12">
+  <conditionalFormatting sqref="J13">
     <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="NOK">
-      <formula>NOT(ISERROR(SEARCH("NOK",J12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J12">
+      <formula>NOT(ISERROR(SEARCH("NOK",J13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J13">
     <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J13">
+  <conditionalFormatting sqref="J14">
     <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="NOK">
-      <formula>NOT(ISERROR(SEARCH("NOK",J13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J13">
+      <formula>NOT(ISERROR(SEARCH("NOK",J14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J14">
     <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J14">
+  <conditionalFormatting sqref="J15">
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="NOK">
-      <formula>NOT(ISERROR(SEARCH("NOK",J14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J14">
+      <formula>NOT(ISERROR(SEARCH("NOK",J15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J15">
+  <conditionalFormatting sqref="J5">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="NOK">
-      <formula>NOT(ISERROR(SEARCH("NOK",J15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J15">
+      <formula>NOT(ISERROR(SEARCH("NOK",J5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>

</xml_diff>